<commit_message>
All testing and data generation complete
</commit_message>
<xml_diff>
--- a/Graph tables.xlsx
+++ b/Graph tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="876" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="876" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="10-40" sheetId="1" r:id="rId1"/>
@@ -16771,7 +16771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B500"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B500"/>
     </sheetView>
   </sheetViews>
@@ -54913,7 +54913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B250"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A244" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A244" workbookViewId="0">
       <selection activeCell="J292" sqref="J292"/>
     </sheetView>
   </sheetViews>

</xml_diff>